<commit_message>
fix: edit county names to include hyphens
</commit_message>
<xml_diff>
--- a/LWCF/Data/StateGrantData/AK_LWCFGrants1965-2011.xlsx
+++ b/LWCF/Data/StateGrantData/AK_LWCFGrants1965-2011.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherkusmierz/GitHub/DataScienceforConservation/LWCF/Data/StateGrantData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFE9773-AB40-D44A-836F-A01F115D1598}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE45834C-7BEB-9F4F-81F6-02DED02B1129}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{B6F33490-F3E6-7A4C-BEE8-2FF3B7EA137C}"/>
+    <workbookView xWindow="19320" yWindow="960" windowWidth="16000" windowHeight="16940" xr2:uid="{B6F33490-F3E6-7A4C-BEE8-2FF3B7EA137C}"/>
   </bookViews>
   <sheets>
     <sheet name="AK" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="649">
   <si>
     <t>Grant ID &amp; Element</t>
   </si>
@@ -999,9 +999,6 @@
     <t>NANCY LAKE WAYSIDE</t>
   </si>
   <si>
-    <t>MATANUSKA SUSITNA</t>
-  </si>
-  <si>
     <t>NANCY LAKE RECREATION AREA</t>
   </si>
   <si>
@@ -1059,9 +1056,6 @@
     <t>CORDOVA MUNICIPAL PARK</t>
   </si>
   <si>
-    <t>VALDEZ CORDOVA</t>
-  </si>
-  <si>
     <t>WEST TENNIS COURT-HOCKEY RINK</t>
   </si>
   <si>
@@ -1503,9 +1497,6 @@
     <t>CITY OF NENANA</t>
   </si>
   <si>
-    <t>YUKON KOYUKUK</t>
-  </si>
-  <si>
     <t>CHENEY LAKE PARK DEVELOPMENT</t>
   </si>
   <si>
@@ -1527,9 +1518,6 @@
     <t>HOMER SPORTSFIELD</t>
   </si>
   <si>
-    <t>KENAI-COOK INLET</t>
-  </si>
-  <si>
     <t>DENALI STATE PARK DEVELOPMENT</t>
   </si>
   <si>
@@ -1974,7 +1962,16 @@
     <t>SKATER'S LAKE PARK</t>
   </si>
   <si>
-    <t>PRINCE OF WALES HYDER</t>
+    <t>PRINCE OF WALES-HYDER</t>
+  </si>
+  <si>
+    <t>MATANUSKA-SUSITNA</t>
+  </si>
+  <si>
+    <t>VALDEZ-CORDOVA</t>
+  </si>
+  <si>
+    <t>YUKON-KOYUKUK</t>
   </si>
 </sst>
 </file>
@@ -2352,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37359A1-6B2A-3F42-BBBF-673668E46398}">
   <dimension ref="A1:I866"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="D162" sqref="D162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2978,7 +2975,7 @@
         <v>288</v>
       </c>
       <c r="D22" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E22" t="s">
         <v>290</v>
@@ -3001,13 +2998,13 @@
         <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C23" t="s">
         <v>288</v>
       </c>
       <c r="D23" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E23" t="s">
         <v>290</v>
@@ -3030,7 +3027,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C24" t="s">
         <v>295</v>
@@ -3056,10 +3053,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>326</v>
+      </c>
+      <c r="B25" t="s">
         <v>327</v>
-      </c>
-      <c r="B25" t="s">
-        <v>328</v>
       </c>
       <c r="C25" t="s">
         <v>307</v>
@@ -3088,13 +3085,13 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C26" t="s">
         <v>288</v>
       </c>
       <c r="D26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E26" t="s">
         <v>290</v>
@@ -3114,10 +3111,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>330</v>
+      </c>
+      <c r="B27" t="s">
         <v>331</v>
-      </c>
-      <c r="B27" t="s">
-        <v>332</v>
       </c>
       <c r="C27" t="s">
         <v>295</v>
@@ -3146,7 +3143,7 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C28" t="s">
         <v>288</v>
@@ -3175,7 +3172,7 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C29" t="s">
         <v>304</v>
@@ -3204,7 +3201,7 @@
         <v>262</v>
       </c>
       <c r="B30" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C30" t="s">
         <v>288</v>
@@ -3233,7 +3230,7 @@
         <v>241</v>
       </c>
       <c r="B31" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C31" t="s">
         <v>293</v>
@@ -3262,7 +3259,7 @@
         <v>244</v>
       </c>
       <c r="B32" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C32" t="s">
         <v>295</v>
@@ -3291,7 +3288,7 @@
         <v>238</v>
       </c>
       <c r="B33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C33" t="s">
         <v>304</v>
@@ -3317,10 +3314,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>338</v>
+      </c>
+      <c r="B34" t="s">
         <v>339</v>
-      </c>
-      <c r="B34" t="s">
-        <v>340</v>
       </c>
       <c r="C34" t="s">
         <v>288</v>
@@ -3349,10 +3346,10 @@
         <v>243</v>
       </c>
       <c r="B35" t="s">
+        <v>340</v>
+      </c>
+      <c r="C35" t="s">
         <v>341</v>
-      </c>
-      <c r="C35" t="s">
-        <v>342</v>
       </c>
       <c r="D35" t="s">
         <v>315</v>
@@ -3378,13 +3375,13 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C36" t="s">
         <v>264</v>
       </c>
       <c r="D36" t="s">
-        <v>344</v>
+        <v>647</v>
       </c>
       <c r="E36" t="s">
         <v>290</v>
@@ -3407,10 +3404,10 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C37" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D37" t="s">
         <v>296</v>
@@ -3436,10 +3433,10 @@
         <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C38" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D38" t="s">
         <v>296</v>
@@ -3465,10 +3462,10 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C39" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D39" t="s">
         <v>296</v>
@@ -3494,10 +3491,10 @@
         <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C40" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D40" t="s">
         <v>296</v>
@@ -3523,7 +3520,7 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C41" t="s">
         <v>295</v>
@@ -3552,7 +3549,7 @@
         <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C42" t="s">
         <v>295</v>
@@ -3581,7 +3578,7 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C43" t="s">
         <v>295</v>
@@ -3610,7 +3607,7 @@
         <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C44" t="s">
         <v>288</v>
@@ -3639,10 +3636,10 @@
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C45" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D45" t="s">
         <v>310</v>
@@ -3668,7 +3665,7 @@
         <v>245</v>
       </c>
       <c r="B46" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C46" t="s">
         <v>288</v>
@@ -3697,10 +3694,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C47" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D47" t="s">
         <v>310</v>
@@ -3726,13 +3723,13 @@
         <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C48" t="s">
         <v>288</v>
       </c>
       <c r="D48" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E48" t="s">
         <v>290</v>
@@ -3755,7 +3752,7 @@
         <v>39</v>
       </c>
       <c r="B49" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C49" t="s">
         <v>288</v>
@@ -3784,7 +3781,7 @@
         <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C50" t="s">
         <v>293</v>
@@ -3813,13 +3810,13 @@
         <v>242</v>
       </c>
       <c r="B51" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C51" t="s">
         <v>264</v>
       </c>
       <c r="D51" t="s">
-        <v>344</v>
+        <v>647</v>
       </c>
       <c r="E51" t="s">
         <v>290</v>
@@ -3842,7 +3839,7 @@
         <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C52" t="s">
         <v>288</v>
@@ -3871,7 +3868,7 @@
         <v>61</v>
       </c>
       <c r="B53" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C53" t="s">
         <v>295</v>
@@ -3900,7 +3897,7 @@
         <v>247</v>
       </c>
       <c r="B54" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C54" t="s">
         <v>295</v>
@@ -3929,7 +3926,7 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C55" t="s">
         <v>295</v>
@@ -3958,7 +3955,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C56" t="s">
         <v>295</v>
@@ -3987,7 +3984,7 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C57" t="s">
         <v>295</v>
@@ -4016,7 +4013,7 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C58" t="s">
         <v>295</v>
@@ -4045,7 +4042,7 @@
         <v>64</v>
       </c>
       <c r="B59" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C59" t="s">
         <v>295</v>
@@ -4074,7 +4071,7 @@
         <v>65</v>
       </c>
       <c r="B60" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C60" t="s">
         <v>295</v>
@@ -4103,7 +4100,7 @@
         <v>66</v>
       </c>
       <c r="B61" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C61" t="s">
         <v>295</v>
@@ -4132,7 +4129,7 @@
         <v>71</v>
       </c>
       <c r="B62" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C62" t="s">
         <v>295</v>
@@ -4158,10 +4155,10 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B63" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C63" t="s">
         <v>302</v>
@@ -4190,7 +4187,7 @@
         <v>50</v>
       </c>
       <c r="B64" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C64" t="s">
         <v>288</v>
@@ -4219,7 +4216,7 @@
         <v>54</v>
       </c>
       <c r="B65" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C65" t="s">
         <v>307</v>
@@ -4248,7 +4245,7 @@
         <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C66" t="s">
         <v>304</v>
@@ -4277,10 +4274,10 @@
         <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C67" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D67" t="s">
         <v>310</v>
@@ -4306,10 +4303,10 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C68" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D68" t="s">
         <v>310</v>
@@ -4335,7 +4332,7 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C69" t="s">
         <v>309</v>
@@ -4364,13 +4361,13 @@
         <v>45</v>
       </c>
       <c r="B70" t="s">
+        <v>380</v>
+      </c>
+      <c r="C70" t="s">
+        <v>381</v>
+      </c>
+      <c r="D70" t="s">
         <v>382</v>
-      </c>
-      <c r="C70" t="s">
-        <v>383</v>
-      </c>
-      <c r="D70" t="s">
-        <v>384</v>
       </c>
       <c r="E70" t="s">
         <v>290</v>
@@ -4393,13 +4390,13 @@
         <v>57</v>
       </c>
       <c r="B71" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C71" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D71" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E71" t="s">
         <v>290</v>
@@ -4422,13 +4419,13 @@
         <v>41</v>
       </c>
       <c r="B72" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C72" t="s">
         <v>288</v>
       </c>
       <c r="D72" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E72" t="s">
         <v>290</v>
@@ -4451,13 +4448,13 @@
         <v>246</v>
       </c>
       <c r="B73" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C73" t="s">
         <v>288</v>
       </c>
       <c r="D73" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E73" t="s">
         <v>290</v>
@@ -4480,13 +4477,13 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C74" t="s">
         <v>288</v>
       </c>
       <c r="D74" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E74" t="s">
         <v>290</v>
@@ -4509,10 +4506,10 @@
         <v>58</v>
       </c>
       <c r="B75" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C75" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D75" t="s">
         <v>315</v>
@@ -4538,13 +4535,13 @@
         <v>53</v>
       </c>
       <c r="B76" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C76" t="s">
         <v>288</v>
       </c>
       <c r="D76" t="s">
-        <v>344</v>
+        <v>647</v>
       </c>
       <c r="E76" t="s">
         <v>290</v>
@@ -4567,13 +4564,13 @@
         <v>68</v>
       </c>
       <c r="B77" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C77" t="s">
         <v>264</v>
       </c>
       <c r="D77" t="s">
-        <v>344</v>
+        <v>647</v>
       </c>
       <c r="E77" t="s">
         <v>290</v>
@@ -4596,7 +4593,7 @@
         <v>72</v>
       </c>
       <c r="B78" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C78" t="s">
         <v>295</v>
@@ -4625,7 +4622,7 @@
         <v>73</v>
       </c>
       <c r="B79" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C79" t="s">
         <v>295</v>
@@ -4654,7 +4651,7 @@
         <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C80" t="s">
         <v>295</v>
@@ -4683,7 +4680,7 @@
         <v>252</v>
       </c>
       <c r="B81" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C81" t="s">
         <v>288</v>
@@ -4712,7 +4709,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C82" t="s">
         <v>295</v>
@@ -4741,7 +4738,7 @@
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C83" t="s">
         <v>295</v>
@@ -4770,7 +4767,7 @@
         <v>253</v>
       </c>
       <c r="B84" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C84" t="s">
         <v>302</v>
@@ -4828,7 +4825,7 @@
         <v>79</v>
       </c>
       <c r="B86" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C86" t="s">
         <v>304</v>
@@ -4857,7 +4854,7 @@
         <v>248</v>
       </c>
       <c r="B87" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C87" t="s">
         <v>288</v>
@@ -4886,7 +4883,7 @@
         <v>249</v>
       </c>
       <c r="B88" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C88" t="s">
         <v>288</v>
@@ -4915,10 +4912,10 @@
         <v>255</v>
       </c>
       <c r="B89" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C89" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D89" t="s">
         <v>310</v>
@@ -4944,13 +4941,13 @@
         <v>78</v>
       </c>
       <c r="B90" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C90" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D90" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E90" t="s">
         <v>290</v>
@@ -4973,13 +4970,13 @@
         <v>75</v>
       </c>
       <c r="B91" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C91" t="s">
         <v>288</v>
       </c>
       <c r="D91" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E91" t="s">
         <v>290</v>
@@ -5002,7 +4999,7 @@
         <v>77</v>
       </c>
       <c r="B92" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C92" t="s">
         <v>288</v>
@@ -5031,13 +5028,13 @@
         <v>82</v>
       </c>
       <c r="B93" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C93" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D93" t="s">
-        <v>344</v>
+        <v>647</v>
       </c>
       <c r="E93" t="s">
         <v>290</v>
@@ -5060,7 +5057,7 @@
         <v>85</v>
       </c>
       <c r="B94" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C94" t="s">
         <v>295</v>
@@ -5089,7 +5086,7 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C95" t="s">
         <v>295</v>
@@ -5118,7 +5115,7 @@
         <v>260</v>
       </c>
       <c r="B96" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C96" t="s">
         <v>295</v>
@@ -5147,7 +5144,7 @@
         <v>257</v>
       </c>
       <c r="B97" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C97" t="s">
         <v>295</v>
@@ -5176,7 +5173,7 @@
         <v>88</v>
       </c>
       <c r="B98" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C98" t="s">
         <v>295</v>
@@ -5205,7 +5202,7 @@
         <v>250</v>
       </c>
       <c r="B99" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C99" t="s">
         <v>295</v>
@@ -5234,7 +5231,7 @@
         <v>86</v>
       </c>
       <c r="B100" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C100" t="s">
         <v>295</v>
@@ -5263,7 +5260,7 @@
         <v>259</v>
       </c>
       <c r="B101" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C101" t="s">
         <v>295</v>
@@ -5292,7 +5289,7 @@
         <v>96</v>
       </c>
       <c r="B102" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C102" t="s">
         <v>302</v>
@@ -5321,7 +5318,7 @@
         <v>97</v>
       </c>
       <c r="B103" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C103" t="s">
         <v>302</v>
@@ -5350,7 +5347,7 @@
         <v>261</v>
       </c>
       <c r="B104" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C104" t="s">
         <v>302</v>
@@ -5379,7 +5376,7 @@
         <v>89</v>
       </c>
       <c r="B105" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C105" t="s">
         <v>302</v>
@@ -5408,7 +5405,7 @@
         <v>258</v>
       </c>
       <c r="B106" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C106" t="s">
         <v>302</v>
@@ -5437,7 +5434,7 @@
         <v>81</v>
       </c>
       <c r="B107" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C107" t="s">
         <v>304</v>
@@ -5466,7 +5463,7 @@
         <v>263</v>
       </c>
       <c r="B108" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C108" t="s">
         <v>304</v>
@@ -5495,10 +5492,10 @@
         <v>93</v>
       </c>
       <c r="B109" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C109" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D109" t="s">
         <v>310</v>
@@ -5524,10 +5521,10 @@
         <v>90</v>
       </c>
       <c r="B110" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C110" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D110" t="s">
         <v>310</v>
@@ -5553,13 +5550,13 @@
         <v>251</v>
       </c>
       <c r="B111" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C111" t="s">
         <v>288</v>
       </c>
       <c r="D111" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E111" t="s">
         <v>290</v>
@@ -5582,7 +5579,7 @@
         <v>254</v>
       </c>
       <c r="B112" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C112" t="s">
         <v>295</v>
@@ -5611,7 +5608,7 @@
         <v>87</v>
       </c>
       <c r="B113" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C113" t="s">
         <v>295</v>
@@ -5640,7 +5637,7 @@
         <v>98</v>
       </c>
       <c r="B114" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C114" t="s">
         <v>295</v>
@@ -5669,7 +5666,7 @@
         <v>92</v>
       </c>
       <c r="B115" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C115" t="s">
         <v>302</v>
@@ -5698,7 +5695,7 @@
         <v>91</v>
       </c>
       <c r="B116" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C116" t="s">
         <v>302</v>
@@ -5727,7 +5724,7 @@
         <v>256</v>
       </c>
       <c r="B117" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C117" t="s">
         <v>304</v>
@@ -5759,7 +5756,7 @@
         <v>265</v>
       </c>
       <c r="C118" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D118" t="s">
         <v>312</v>
@@ -5785,13 +5782,13 @@
         <v>110</v>
       </c>
       <c r="B119" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C119" t="s">
         <v>288</v>
       </c>
       <c r="D119" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E119" t="s">
         <v>290</v>
@@ -5814,7 +5811,7 @@
         <v>108</v>
       </c>
       <c r="B120" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C120" t="s">
         <v>295</v>
@@ -5843,7 +5840,7 @@
         <v>104</v>
       </c>
       <c r="B121" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C121" t="s">
         <v>295</v>
@@ -5872,7 +5869,7 @@
         <v>100</v>
       </c>
       <c r="B122" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C122" t="s">
         <v>295</v>
@@ -5901,7 +5898,7 @@
         <v>109</v>
       </c>
       <c r="B123" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C123" t="s">
         <v>295</v>
@@ -5930,7 +5927,7 @@
         <v>99</v>
       </c>
       <c r="B124" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C124" t="s">
         <v>302</v>
@@ -5959,7 +5956,7 @@
         <v>105</v>
       </c>
       <c r="B125" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C125" t="s">
         <v>302</v>
@@ -5988,7 +5985,7 @@
         <v>112</v>
       </c>
       <c r="B126" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C126" t="s">
         <v>302</v>
@@ -6017,10 +6014,10 @@
         <v>266</v>
       </c>
       <c r="B127" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C127" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D127" t="s">
         <v>320</v>
@@ -6046,7 +6043,7 @@
         <v>102</v>
       </c>
       <c r="B128" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C128" t="s">
         <v>304</v>
@@ -6075,10 +6072,10 @@
         <v>103</v>
       </c>
       <c r="B129" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C129" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D129" t="s">
         <v>310</v>
@@ -6104,13 +6101,13 @@
         <v>111</v>
       </c>
       <c r="B130" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C130" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D130" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E130" t="s">
         <v>290</v>
@@ -6133,13 +6130,13 @@
         <v>101</v>
       </c>
       <c r="B131" t="s">
+        <v>442</v>
+      </c>
+      <c r="C131" t="s">
+        <v>443</v>
+      </c>
+      <c r="D131" t="s">
         <v>444</v>
-      </c>
-      <c r="C131" t="s">
-        <v>445</v>
-      </c>
-      <c r="D131" t="s">
-        <v>446</v>
       </c>
       <c r="E131" t="s">
         <v>290</v>
@@ -6159,10 +6156,10 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B132" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C132" t="s">
         <v>293</v>
@@ -6191,7 +6188,7 @@
         <v>106</v>
       </c>
       <c r="B133" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C133" t="s">
         <v>288</v>
@@ -6220,7 +6217,7 @@
         <v>118</v>
       </c>
       <c r="B134" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C134" t="s">
         <v>295</v>
@@ -6249,7 +6246,7 @@
         <v>270</v>
       </c>
       <c r="B135" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C135" t="s">
         <v>288</v>
@@ -6275,16 +6272,16 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B136" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C136" t="s">
         <v>288</v>
       </c>
       <c r="D136" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E136" t="s">
         <v>290</v>
@@ -6307,13 +6304,13 @@
         <v>107</v>
       </c>
       <c r="B137" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C137" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D137" t="s">
-        <v>344</v>
+        <v>647</v>
       </c>
       <c r="E137" t="s">
         <v>290</v>
@@ -6336,13 +6333,13 @@
         <v>115</v>
       </c>
       <c r="B138" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C138" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D138" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E138" t="s">
         <v>290</v>
@@ -6365,13 +6362,13 @@
         <v>117</v>
       </c>
       <c r="B139" t="s">
+        <v>455</v>
+      </c>
+      <c r="C139" t="s">
+        <v>456</v>
+      </c>
+      <c r="D139" t="s">
         <v>457</v>
-      </c>
-      <c r="C139" t="s">
-        <v>458</v>
-      </c>
-      <c r="D139" t="s">
-        <v>459</v>
       </c>
       <c r="E139" t="s">
         <v>290</v>
@@ -6394,10 +6391,10 @@
         <v>269</v>
       </c>
       <c r="B140" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C140" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D140" t="s">
         <v>320</v>
@@ -6423,7 +6420,7 @@
         <v>113</v>
       </c>
       <c r="B141" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C141" t="s">
         <v>304</v>
@@ -6452,7 +6449,7 @@
         <v>123</v>
       </c>
       <c r="B142" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C142" t="s">
         <v>304</v>
@@ -6481,7 +6478,7 @@
         <v>120</v>
       </c>
       <c r="B143" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C143" t="s">
         <v>288</v>
@@ -6510,7 +6507,7 @@
         <v>116</v>
       </c>
       <c r="B144" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C144" t="s">
         <v>288</v>
@@ -6539,7 +6536,7 @@
         <v>127</v>
       </c>
       <c r="B145" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C145" t="s">
         <v>288</v>
@@ -6597,13 +6594,13 @@
         <v>119</v>
       </c>
       <c r="B147" t="s">
+        <v>464</v>
+      </c>
+      <c r="C147" t="s">
+        <v>465</v>
+      </c>
+      <c r="D147" t="s">
         <v>466</v>
-      </c>
-      <c r="C147" t="s">
-        <v>467</v>
-      </c>
-      <c r="D147" t="s">
-        <v>468</v>
       </c>
       <c r="E147" t="s">
         <v>290</v>
@@ -6626,13 +6623,13 @@
         <v>271</v>
       </c>
       <c r="B148" t="s">
+        <v>467</v>
+      </c>
+      <c r="C148" t="s">
+        <v>468</v>
+      </c>
+      <c r="D148" t="s">
         <v>469</v>
-      </c>
-      <c r="C148" t="s">
-        <v>470</v>
-      </c>
-      <c r="D148" t="s">
-        <v>471</v>
       </c>
       <c r="E148" t="s">
         <v>290</v>
@@ -6655,7 +6652,7 @@
         <v>124</v>
       </c>
       <c r="B149" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C149" t="s">
         <v>288</v>
@@ -6684,13 +6681,13 @@
         <v>126</v>
       </c>
       <c r="B150" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C150" t="s">
         <v>264</v>
       </c>
       <c r="D150" t="s">
-        <v>344</v>
+        <v>647</v>
       </c>
       <c r="E150" t="s">
         <v>290</v>
@@ -6713,7 +6710,7 @@
         <v>267</v>
       </c>
       <c r="B151" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C151" t="s">
         <v>295</v>
@@ -6742,7 +6739,7 @@
         <v>268</v>
       </c>
       <c r="B152" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C152" t="s">
         <v>295</v>
@@ -6771,7 +6768,7 @@
         <v>139</v>
       </c>
       <c r="B153" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C153" t="s">
         <v>288</v>
@@ -6800,10 +6797,10 @@
         <v>141</v>
       </c>
       <c r="B154" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C154" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D154" t="s">
         <v>310</v>
@@ -6829,7 +6826,7 @@
         <v>144</v>
       </c>
       <c r="B155" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C155" t="s">
         <v>288</v>
@@ -6858,10 +6855,10 @@
         <v>128</v>
       </c>
       <c r="B156" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C156" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D156" t="s">
         <v>312</v>
@@ -6887,10 +6884,10 @@
         <v>152</v>
       </c>
       <c r="B157" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C157" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D157" t="s">
         <v>312</v>
@@ -6916,13 +6913,13 @@
         <v>122</v>
       </c>
       <c r="B158" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C158" t="s">
         <v>288</v>
       </c>
       <c r="D158" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E158" t="s">
         <v>290</v>
@@ -6945,13 +6942,13 @@
         <v>135</v>
       </c>
       <c r="B159" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C159" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D159" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E159" t="s">
         <v>290</v>
@@ -6974,13 +6971,13 @@
         <v>272</v>
       </c>
       <c r="B160" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C160" t="s">
         <v>288</v>
       </c>
       <c r="D160" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E160" t="s">
         <v>290</v>
@@ -7003,13 +7000,13 @@
         <v>121</v>
       </c>
       <c r="B161" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C161" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D161" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E161" t="s">
         <v>290</v>
@@ -7029,16 +7026,16 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
+        <v>484</v>
+      </c>
+      <c r="B162" t="s">
+        <v>485</v>
+      </c>
+      <c r="C162" t="s">
         <v>486</v>
       </c>
-      <c r="B162" t="s">
+      <c r="D162" t="s">
         <v>487</v>
-      </c>
-      <c r="C162" t="s">
-        <v>488</v>
-      </c>
-      <c r="D162" t="s">
-        <v>489</v>
       </c>
       <c r="E162" t="s">
         <v>290</v>
@@ -7061,13 +7058,13 @@
         <v>125</v>
       </c>
       <c r="B163" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C163" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D163" t="s">
-        <v>492</v>
+        <v>648</v>
       </c>
       <c r="E163" t="s">
         <v>290</v>
@@ -7090,7 +7087,7 @@
         <v>132</v>
       </c>
       <c r="B164" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C164" t="s">
         <v>295</v>
@@ -7119,7 +7116,7 @@
         <v>133</v>
       </c>
       <c r="B165" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C165" t="s">
         <v>295</v>
@@ -7148,7 +7145,7 @@
         <v>136</v>
       </c>
       <c r="B166" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C166" t="s">
         <v>295</v>
@@ -7177,7 +7174,7 @@
         <v>150</v>
       </c>
       <c r="B167" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C167" t="s">
         <v>295</v>
@@ -7206,7 +7203,7 @@
         <v>143</v>
       </c>
       <c r="B168" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C168" t="s">
         <v>295</v>
@@ -7235,7 +7232,7 @@
         <v>131</v>
       </c>
       <c r="B169" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C169" t="s">
         <v>288</v>
@@ -7264,13 +7261,13 @@
         <v>140</v>
       </c>
       <c r="B170" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C170" t="s">
         <v>288</v>
       </c>
       <c r="D170" t="s">
-        <v>500</v>
+        <v>310</v>
       </c>
       <c r="E170" t="s">
         <v>290</v>
@@ -7293,13 +7290,13 @@
         <v>145</v>
       </c>
       <c r="B171" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C171" t="s">
         <v>288</v>
       </c>
       <c r="D171" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E171" t="s">
         <v>290</v>
@@ -7322,13 +7319,13 @@
         <v>153</v>
       </c>
       <c r="B172" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C172" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D172" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E172" t="s">
         <v>290</v>
@@ -7351,13 +7348,13 @@
         <v>273</v>
       </c>
       <c r="B173" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C173" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D173" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E173" t="s">
         <v>290</v>
@@ -7380,13 +7377,13 @@
         <v>137</v>
       </c>
       <c r="B174" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C174" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D174" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E174" t="s">
         <v>290</v>
@@ -7409,13 +7406,13 @@
         <v>146</v>
       </c>
       <c r="B175" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="C175" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D175" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E175" t="s">
         <v>290</v>
@@ -7438,7 +7435,7 @@
         <v>134</v>
       </c>
       <c r="B176" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="C176" t="s">
         <v>288</v>
@@ -7467,13 +7464,13 @@
         <v>275</v>
       </c>
       <c r="B177" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C177" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D177" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E177" t="s">
         <v>290</v>
@@ -7496,13 +7493,13 @@
         <v>148</v>
       </c>
       <c r="B178" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="C178" t="s">
         <v>264</v>
       </c>
       <c r="D178" t="s">
-        <v>344</v>
+        <v>647</v>
       </c>
       <c r="E178" t="s">
         <v>290</v>
@@ -7525,13 +7522,13 @@
         <v>151</v>
       </c>
       <c r="B179" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C179" t="s">
         <v>264</v>
       </c>
       <c r="D179" t="s">
-        <v>344</v>
+        <v>647</v>
       </c>
       <c r="E179" t="s">
         <v>290</v>
@@ -7554,13 +7551,13 @@
         <v>274</v>
       </c>
       <c r="B180" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C180" t="s">
         <v>264</v>
       </c>
       <c r="D180" t="s">
-        <v>344</v>
+        <v>647</v>
       </c>
       <c r="E180" t="s">
         <v>290</v>
@@ -7583,13 +7580,13 @@
         <v>149</v>
       </c>
       <c r="B181" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C181" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D181" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E181" t="s">
         <v>290</v>
@@ -7612,13 +7609,13 @@
         <v>129</v>
       </c>
       <c r="B182" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C182" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D182" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="E182" t="s">
         <v>290</v>
@@ -7641,13 +7638,13 @@
         <v>159</v>
       </c>
       <c r="B183" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="C183" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="D183" t="s">
-        <v>492</v>
+        <v>648</v>
       </c>
       <c r="E183" t="s">
         <v>290</v>
@@ -7670,7 +7667,7 @@
         <v>175</v>
       </c>
       <c r="B184" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C184" t="s">
         <v>295</v>
@@ -7699,10 +7696,10 @@
         <v>176</v>
       </c>
       <c r="B185" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="C185" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D185" t="s">
         <v>310</v>
@@ -7728,13 +7725,13 @@
         <v>138</v>
       </c>
       <c r="B186" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="C186" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D186" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E186" t="s">
         <v>290</v>
@@ -7757,7 +7754,7 @@
         <v>161</v>
       </c>
       <c r="B187" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C187" t="s">
         <v>288</v>
@@ -7786,13 +7783,13 @@
         <v>276</v>
       </c>
       <c r="B188" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C188" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D188" t="s">
-        <v>344</v>
+        <v>647</v>
       </c>
       <c r="E188" t="s">
         <v>290</v>
@@ -7812,16 +7809,16 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B189" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C189" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D189" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="E189" t="s">
         <v>290</v>
@@ -7844,13 +7841,13 @@
         <v>147</v>
       </c>
       <c r="B190" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="C190" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D190" t="s">
-        <v>492</v>
+        <v>648</v>
       </c>
       <c r="E190" t="s">
         <v>290</v>
@@ -7873,7 +7870,7 @@
         <v>154</v>
       </c>
       <c r="B191" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C191" t="s">
         <v>295</v>
@@ -7902,10 +7899,10 @@
         <v>155</v>
       </c>
       <c r="B192" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="C192" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D192" t="s">
         <v>310</v>
@@ -7931,10 +7928,10 @@
         <v>163</v>
       </c>
       <c r="B193" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="C193" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D193" t="s">
         <v>320</v>
@@ -7960,7 +7957,7 @@
         <v>162</v>
       </c>
       <c r="B194" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C194" t="s">
         <v>304</v>
@@ -7989,13 +7986,13 @@
         <v>177</v>
       </c>
       <c r="B195" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C195" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D195" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E195" t="s">
         <v>290</v>
@@ -8018,13 +8015,13 @@
         <v>164</v>
       </c>
       <c r="B196" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="C196" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D196" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="E196" t="s">
         <v>290</v>
@@ -8047,7 +8044,7 @@
         <v>172</v>
       </c>
       <c r="B197" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C197" t="s">
         <v>288</v>
@@ -8076,13 +8073,13 @@
         <v>156</v>
       </c>
       <c r="B198" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="C198" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D198" t="s">
-        <v>344</v>
+        <v>647</v>
       </c>
       <c r="E198" t="s">
         <v>290</v>
@@ -8105,7 +8102,7 @@
         <v>173</v>
       </c>
       <c r="B199" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="C199" t="s">
         <v>288</v>
@@ -8134,13 +8131,13 @@
         <v>178</v>
       </c>
       <c r="B200" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="C200" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D200" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E200" t="s">
         <v>290</v>
@@ -8163,13 +8160,13 @@
         <v>166</v>
       </c>
       <c r="B201" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="C201" t="s">
         <v>288</v>
       </c>
       <c r="D201" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E201" t="s">
         <v>290</v>
@@ -8189,13 +8186,13 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="B202" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C202" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D202" t="s">
         <v>49</v>
@@ -8221,7 +8218,7 @@
         <v>167</v>
       </c>
       <c r="B203" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C203" t="s">
         <v>293</v>
@@ -8250,13 +8247,13 @@
         <v>165</v>
       </c>
       <c r="B204" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C204" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="D204" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="E204" t="s">
         <v>290</v>
@@ -8279,13 +8276,13 @@
         <v>169</v>
       </c>
       <c r="B205" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="C205" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D205" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E205" t="s">
         <v>290</v>
@@ -8308,7 +8305,7 @@
         <v>174</v>
       </c>
       <c r="B206" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C206" t="s">
         <v>288</v>
@@ -8337,10 +8334,10 @@
         <v>158</v>
       </c>
       <c r="B207" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C207" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D207" t="s">
         <v>312</v>
@@ -8366,13 +8363,13 @@
         <v>179</v>
       </c>
       <c r="B208" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C208" t="s">
         <v>288</v>
       </c>
       <c r="D208" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E208" t="s">
         <v>290</v>
@@ -8395,13 +8392,13 @@
         <v>157</v>
       </c>
       <c r="B209" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C209" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D209" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E209" t="s">
         <v>290</v>
@@ -8424,13 +8421,13 @@
         <v>171</v>
       </c>
       <c r="B210" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="C210" t="s">
         <v>288</v>
       </c>
       <c r="D210" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E210" t="s">
         <v>290</v>
@@ -8453,13 +8450,13 @@
         <v>170</v>
       </c>
       <c r="B211" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C211" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D211" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E211" t="s">
         <v>290</v>
@@ -8482,13 +8479,13 @@
         <v>168</v>
       </c>
       <c r="B212" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C212" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D212" t="s">
-        <v>492</v>
+        <v>648</v>
       </c>
       <c r="E212" t="s">
         <v>290</v>
@@ -8511,7 +8508,7 @@
         <v>184</v>
       </c>
       <c r="B213" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C213" t="s">
         <v>295</v>
@@ -8537,13 +8534,13 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B214" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C214" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D214" t="s">
         <v>310</v>
@@ -8569,10 +8566,10 @@
         <v>189</v>
       </c>
       <c r="B215" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C215" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D215" t="s">
         <v>310</v>
@@ -8598,13 +8595,13 @@
         <v>190</v>
       </c>
       <c r="B216" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="C216" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D216" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E216" t="s">
         <v>290</v>
@@ -8627,13 +8624,13 @@
         <v>188</v>
       </c>
       <c r="B217" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C217" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D217" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E217" t="s">
         <v>290</v>
@@ -8656,13 +8653,13 @@
         <v>180</v>
       </c>
       <c r="B218" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C218" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="D218" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E218" t="s">
         <v>290</v>
@@ -8685,13 +8682,13 @@
         <v>186</v>
       </c>
       <c r="B219" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C219" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="D219" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E219" t="s">
         <v>290</v>
@@ -8714,7 +8711,7 @@
         <v>185</v>
       </c>
       <c r="B220" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C220" t="s">
         <v>293</v>
@@ -8743,13 +8740,13 @@
         <v>187</v>
       </c>
       <c r="B221" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C221" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D221" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="E221" t="s">
         <v>290</v>
@@ -8772,7 +8769,7 @@
         <v>183</v>
       </c>
       <c r="B222" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C222" t="s">
         <v>288</v>
@@ -8801,10 +8798,10 @@
         <v>181</v>
       </c>
       <c r="B223" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="C223" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D223" t="s">
         <v>310</v>
@@ -8830,13 +8827,13 @@
         <v>191</v>
       </c>
       <c r="B224" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C224" t="s">
         <v>288</v>
       </c>
       <c r="D224" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E224" t="s">
         <v>290</v>
@@ -8859,7 +8856,7 @@
         <v>277</v>
       </c>
       <c r="B225" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C225" t="s">
         <v>293</v>
@@ -8888,13 +8885,13 @@
         <v>182</v>
       </c>
       <c r="B226" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C226" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D226" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E226" t="s">
         <v>290</v>
@@ -8917,7 +8914,7 @@
         <v>193</v>
       </c>
       <c r="B227" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="C227" t="s">
         <v>288</v>
@@ -8946,13 +8943,13 @@
         <v>198</v>
       </c>
       <c r="B228" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C228" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D228" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E228" t="s">
         <v>290</v>
@@ -8975,13 +8972,13 @@
         <v>202</v>
       </c>
       <c r="B229" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="C229" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D229" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E229" t="s">
         <v>290</v>
@@ -9004,7 +9001,7 @@
         <v>192</v>
       </c>
       <c r="B230" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C230" t="s">
         <v>293</v>
@@ -9036,7 +9033,7 @@
         <v>130</v>
       </c>
       <c r="C231" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="D231" t="s">
         <v>310</v>
@@ -9062,7 +9059,7 @@
         <v>282</v>
       </c>
       <c r="B232" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C232" t="s">
         <v>288</v>
@@ -9091,13 +9088,13 @@
         <v>203</v>
       </c>
       <c r="B233" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="C233" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="D233" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E233" t="s">
         <v>290</v>
@@ -9120,13 +9117,13 @@
         <v>194</v>
       </c>
       <c r="B234" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="C234" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D234" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E234" t="s">
         <v>290</v>
@@ -9149,13 +9146,13 @@
         <v>285</v>
       </c>
       <c r="B235" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="C235" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D235" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E235" t="s">
         <v>290</v>
@@ -9178,13 +9175,13 @@
         <v>208</v>
       </c>
       <c r="B236" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="C236" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D236" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E236" t="s">
         <v>290</v>
@@ -9207,13 +9204,13 @@
         <v>200</v>
       </c>
       <c r="B237" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="C237" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D237" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="E237" t="s">
         <v>290</v>
@@ -9236,10 +9233,10 @@
         <v>206</v>
       </c>
       <c r="B238" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="C238" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="D238" t="s">
         <v>310</v>
@@ -9265,13 +9262,13 @@
         <v>195</v>
       </c>
       <c r="B239" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C239" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D239" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E239" t="s">
         <v>290</v>
@@ -9294,13 +9291,13 @@
         <v>199</v>
       </c>
       <c r="B240" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="C240" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D240" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E240" t="s">
         <v>290</v>
@@ -9323,13 +9320,13 @@
         <v>201</v>
       </c>
       <c r="B241" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="C241" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="D241" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E241" t="s">
         <v>290</v>
@@ -9352,10 +9349,10 @@
         <v>207</v>
       </c>
       <c r="B242" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C242" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="D242" t="s">
         <v>312</v>
@@ -9381,13 +9378,13 @@
         <v>205</v>
       </c>
       <c r="B243" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C243" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D243" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E243" t="s">
         <v>290</v>
@@ -9410,7 +9407,7 @@
         <v>197</v>
       </c>
       <c r="B244" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="C244" t="s">
         <v>293</v>
@@ -9439,10 +9436,10 @@
         <v>196</v>
       </c>
       <c r="B245" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C245" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D245" t="s">
         <v>315</v>
@@ -9468,7 +9465,7 @@
         <v>280</v>
       </c>
       <c r="B246" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="C246" t="s">
         <v>293</v>
@@ -9497,7 +9494,7 @@
         <v>209</v>
       </c>
       <c r="B247" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="C247" t="s">
         <v>288</v>
@@ -9526,10 +9523,10 @@
         <v>214</v>
       </c>
       <c r="B248" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="C248" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D248" t="s">
         <v>310</v>
@@ -9555,7 +9552,7 @@
         <v>213</v>
       </c>
       <c r="B249" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="C249" t="s">
         <v>288</v>
@@ -9584,7 +9581,7 @@
         <v>281</v>
       </c>
       <c r="B250" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C250" t="s">
         <v>304</v>
@@ -9613,7 +9610,7 @@
         <v>212</v>
       </c>
       <c r="B251" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="C251" t="s">
         <v>288</v>
@@ -9642,7 +9639,7 @@
         <v>216</v>
       </c>
       <c r="B252" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="C252" t="s">
         <v>288</v>
@@ -9671,10 +9668,10 @@
         <v>283</v>
       </c>
       <c r="B253" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C253" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D253" t="s">
         <v>320</v>
@@ -9700,7 +9697,7 @@
         <v>211</v>
       </c>
       <c r="B254" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C254" t="s">
         <v>288</v>
@@ -9729,7 +9726,7 @@
         <v>284</v>
       </c>
       <c r="B255" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="C255" t="s">
         <v>288</v>
@@ -9758,7 +9755,7 @@
         <v>210</v>
       </c>
       <c r="B256" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="C256" t="s">
         <v>293</v>
@@ -9787,10 +9784,10 @@
         <v>219</v>
       </c>
       <c r="B257" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C257" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D257" t="s">
         <v>315</v>
@@ -9816,13 +9813,13 @@
         <v>220</v>
       </c>
       <c r="B258" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="C258" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D258" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E258" t="s">
         <v>290</v>
@@ -9845,13 +9842,13 @@
         <v>215</v>
       </c>
       <c r="B259" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C259" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D259" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E259" t="s">
         <v>290</v>
@@ -9874,7 +9871,7 @@
         <v>279</v>
       </c>
       <c r="B260" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C260" t="s">
         <v>302</v>
@@ -9903,10 +9900,10 @@
         <v>278</v>
       </c>
       <c r="B261" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C261" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D261" t="s">
         <v>310</v>
@@ -9932,7 +9929,7 @@
         <v>225</v>
       </c>
       <c r="B262" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="C262" t="s">
         <v>293</v>
@@ -9961,7 +9958,7 @@
         <v>218</v>
       </c>
       <c r="B263" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="C263" t="s">
         <v>288</v>
@@ -9990,7 +9987,7 @@
         <v>224</v>
       </c>
       <c r="B264" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C264" t="s">
         <v>288</v>
@@ -10019,13 +10016,13 @@
         <v>222</v>
       </c>
       <c r="B265" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C265" t="s">
         <v>288</v>
       </c>
       <c r="D265" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E265" t="s">
         <v>290</v>
@@ -10048,13 +10045,13 @@
         <v>229</v>
       </c>
       <c r="B266" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="C266" t="s">
         <v>288</v>
       </c>
       <c r="D266" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E266" t="s">
         <v>290</v>
@@ -10077,13 +10074,13 @@
         <v>217</v>
       </c>
       <c r="B267" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="C267" t="s">
         <v>264</v>
       </c>
       <c r="D267" t="s">
-        <v>344</v>
+        <v>647</v>
       </c>
       <c r="E267" t="s">
         <v>290</v>
@@ -10106,7 +10103,7 @@
         <v>221</v>
       </c>
       <c r="B268" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="C268" t="s">
         <v>288</v>
@@ -10135,7 +10132,7 @@
         <v>223</v>
       </c>
       <c r="B269" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="C269" t="s">
         <v>302</v>
@@ -10164,13 +10161,13 @@
         <v>230</v>
       </c>
       <c r="B270" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="C270" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="D270" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="E270" t="s">
         <v>290</v>
@@ -10193,10 +10190,10 @@
         <v>233</v>
       </c>
       <c r="B271" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="C271" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D271" t="s">
         <v>315</v>
@@ -10222,7 +10219,7 @@
         <v>232</v>
       </c>
       <c r="B272" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="C272" t="s">
         <v>288</v>
@@ -10251,7 +10248,7 @@
         <v>227</v>
       </c>
       <c r="B273" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C273" t="s">
         <v>304</v>
@@ -10280,7 +10277,7 @@
         <v>226</v>
       </c>
       <c r="B274" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="C274" t="s">
         <v>288</v>
@@ -10309,13 +10306,13 @@
         <v>231</v>
       </c>
       <c r="B275" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="C275" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="D275" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="E275" t="s">
         <v>290</v>
@@ -10338,7 +10335,7 @@
         <v>235</v>
       </c>
       <c r="B276" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C276" t="s">
         <v>302</v>
@@ -10367,10 +10364,10 @@
         <v>286</v>
       </c>
       <c r="B277" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C277" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D277" t="s">
         <v>310</v>
@@ -10396,7 +10393,7 @@
         <v>234</v>
       </c>
       <c r="B278" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="C278" t="s">
         <v>288</v>
@@ -10425,13 +10422,13 @@
         <v>228</v>
       </c>
       <c r="B279" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C279" t="s">
         <v>288</v>
       </c>
       <c r="D279" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="E279" t="s">
         <v>290</v>
@@ -10451,16 +10448,16 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="B280" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="C280" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D280" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="E280" t="s">
         <v>290</v>

</xml_diff>

<commit_message>
fix: update county info to match county id data
</commit_message>
<xml_diff>
--- a/LWCF/Data/StateGrantData/AK_LWCFGrants1965-2011.xlsx
+++ b/LWCF/Data/StateGrantData/AK_LWCFGrants1965-2011.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherkusmierz/GitHub/DataScienceforConservation/LWCF/Data/StateGrantData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE45834C-7BEB-9F4F-81F6-02DED02B1129}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2D0A93-964D-C044-8D03-A759E7286DC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19320" yWindow="960" windowWidth="16000" windowHeight="16940" xr2:uid="{B6F33490-F3E6-7A4C-BEE8-2FF3B7EA137C}"/>
+    <workbookView xWindow="17600" yWindow="960" windowWidth="16000" windowHeight="16940" xr2:uid="{B6F33490-F3E6-7A4C-BEE8-2FF3B7EA137C}"/>
   </bookViews>
   <sheets>
     <sheet name="AK" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="647">
   <si>
     <t>Grant ID &amp; Element</t>
   </si>
@@ -1434,9 +1434,6 @@
     <t>METLAKATLA INDIAN COMMUNITY</t>
   </si>
   <si>
-    <t>PRINCE WALES KETCHIKAN</t>
-  </si>
-  <si>
     <t>HALIBUT POINT WAYSIDE</t>
   </si>
   <si>
@@ -1476,9 +1473,6 @@
     <t>ALPINE WOODS NEIGHBORHOOD PARK</t>
   </si>
   <si>
-    <t>VALDEZ-CHITINA-W</t>
-  </si>
-  <si>
     <t>267 - XXX</t>
   </si>
   <si>
@@ -1488,9 +1482,6 @@
     <t>CITY OF PETERSBURG</t>
   </si>
   <si>
-    <t>WRANGELL PETERSBURG</t>
-  </si>
-  <si>
     <t>CITY PARKS</t>
   </si>
   <si>
@@ -1972,6 +1963,9 @@
   </si>
   <si>
     <t>YUKON-KOYUKUK</t>
+  </si>
+  <si>
+    <t>PETERSBURG</t>
   </si>
 </sst>
 </file>
@@ -2006,12 +2000,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2027,11 +2027,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2349,9 +2350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37359A1-6B2A-3F42-BBBF-673668E46398}">
   <dimension ref="A1:I866"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="D162" sqref="D162"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2975,7 +2974,7 @@
         <v>288</v>
       </c>
       <c r="D22" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E22" t="s">
         <v>290</v>
@@ -3004,7 +3003,7 @@
         <v>288</v>
       </c>
       <c r="D23" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E23" t="s">
         <v>290</v>
@@ -3381,7 +3380,7 @@
         <v>264</v>
       </c>
       <c r="D36" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E36" t="s">
         <v>290</v>
@@ -3729,7 +3728,7 @@
         <v>288</v>
       </c>
       <c r="D48" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E48" t="s">
         <v>290</v>
@@ -3816,7 +3815,7 @@
         <v>264</v>
       </c>
       <c r="D51" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E51" t="s">
         <v>290</v>
@@ -4425,7 +4424,7 @@
         <v>288</v>
       </c>
       <c r="D72" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E72" t="s">
         <v>290</v>
@@ -4454,7 +4453,7 @@
         <v>288</v>
       </c>
       <c r="D73" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E73" t="s">
         <v>290</v>
@@ -4483,7 +4482,7 @@
         <v>288</v>
       </c>
       <c r="D74" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E74" t="s">
         <v>290</v>
@@ -4541,7 +4540,7 @@
         <v>288</v>
       </c>
       <c r="D76" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E76" t="s">
         <v>290</v>
@@ -4570,7 +4569,7 @@
         <v>264</v>
       </c>
       <c r="D77" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E77" t="s">
         <v>290</v>
@@ -4976,7 +4975,7 @@
         <v>288</v>
       </c>
       <c r="D91" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E91" t="s">
         <v>290</v>
@@ -5034,7 +5033,7 @@
         <v>404</v>
       </c>
       <c r="D93" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E93" t="s">
         <v>290</v>
@@ -5556,7 +5555,7 @@
         <v>288</v>
       </c>
       <c r="D111" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E111" t="s">
         <v>290</v>
@@ -6281,7 +6280,7 @@
         <v>288</v>
       </c>
       <c r="D136" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E136" t="s">
         <v>290</v>
@@ -6310,7 +6309,7 @@
         <v>404</v>
       </c>
       <c r="D137" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E137" t="s">
         <v>290</v>
@@ -6628,8 +6627,8 @@
       <c r="C148" t="s">
         <v>468</v>
       </c>
-      <c r="D148" t="s">
-        <v>469</v>
+      <c r="D148" s="4" t="s">
+        <v>312</v>
       </c>
       <c r="E148" t="s">
         <v>290</v>
@@ -6652,7 +6651,7 @@
         <v>124</v>
       </c>
       <c r="B149" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C149" t="s">
         <v>288</v>
@@ -6681,13 +6680,13 @@
         <v>126</v>
       </c>
       <c r="B150" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C150" t="s">
         <v>264</v>
       </c>
       <c r="D150" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E150" t="s">
         <v>290</v>
@@ -6710,7 +6709,7 @@
         <v>267</v>
       </c>
       <c r="B151" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C151" t="s">
         <v>295</v>
@@ -6739,7 +6738,7 @@
         <v>268</v>
       </c>
       <c r="B152" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C152" t="s">
         <v>295</v>
@@ -6768,7 +6767,7 @@
         <v>139</v>
       </c>
       <c r="B153" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C153" t="s">
         <v>288</v>
@@ -6797,7 +6796,7 @@
         <v>141</v>
       </c>
       <c r="B154" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C154" t="s">
         <v>355</v>
@@ -6826,7 +6825,7 @@
         <v>144</v>
       </c>
       <c r="B155" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C155" t="s">
         <v>288</v>
@@ -6855,7 +6854,7 @@
         <v>128</v>
       </c>
       <c r="B156" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C156" t="s">
         <v>429</v>
@@ -6884,7 +6883,7 @@
         <v>152</v>
       </c>
       <c r="B157" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C157" t="s">
         <v>429</v>
@@ -6913,7 +6912,7 @@
         <v>122</v>
       </c>
       <c r="B158" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C158" t="s">
         <v>288</v>
@@ -6942,7 +6941,7 @@
         <v>135</v>
       </c>
       <c r="B159" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C159" t="s">
         <v>381</v>
@@ -6971,13 +6970,13 @@
         <v>272</v>
       </c>
       <c r="B160" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C160" t="s">
         <v>288</v>
       </c>
       <c r="D160" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E160" t="s">
         <v>290</v>
@@ -7000,13 +6999,13 @@
         <v>121</v>
       </c>
       <c r="B161" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C161" t="s">
         <v>404</v>
       </c>
-      <c r="D161" t="s">
-        <v>483</v>
+      <c r="D161" s="4" t="s">
+        <v>644</v>
       </c>
       <c r="E161" t="s">
         <v>290</v>
@@ -7026,16 +7025,16 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
+        <v>482</v>
+      </c>
+      <c r="B162" t="s">
+        <v>483</v>
+      </c>
+      <c r="C162" t="s">
         <v>484</v>
       </c>
-      <c r="B162" t="s">
-        <v>485</v>
-      </c>
-      <c r="C162" t="s">
-        <v>486</v>
-      </c>
-      <c r="D162" t="s">
-        <v>487</v>
+      <c r="D162" s="4" t="s">
+        <v>646</v>
       </c>
       <c r="E162" t="s">
         <v>290</v>
@@ -7058,13 +7057,13 @@
         <v>125</v>
       </c>
       <c r="B163" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C163" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D163" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="E163" t="s">
         <v>290</v>
@@ -7087,7 +7086,7 @@
         <v>132</v>
       </c>
       <c r="B164" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C164" t="s">
         <v>295</v>
@@ -7116,7 +7115,7 @@
         <v>133</v>
       </c>
       <c r="B165" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C165" t="s">
         <v>295</v>
@@ -7145,7 +7144,7 @@
         <v>136</v>
       </c>
       <c r="B166" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C166" t="s">
         <v>295</v>
@@ -7174,7 +7173,7 @@
         <v>150</v>
       </c>
       <c r="B167" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C167" t="s">
         <v>295</v>
@@ -7203,7 +7202,7 @@
         <v>143</v>
       </c>
       <c r="B168" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C168" t="s">
         <v>295</v>
@@ -7232,7 +7231,7 @@
         <v>131</v>
       </c>
       <c r="B169" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C169" t="s">
         <v>288</v>
@@ -7261,7 +7260,7 @@
         <v>140</v>
       </c>
       <c r="B170" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C170" t="s">
         <v>288</v>
@@ -7290,13 +7289,13 @@
         <v>145</v>
       </c>
       <c r="B171" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C171" t="s">
         <v>288</v>
       </c>
       <c r="D171" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E171" t="s">
         <v>290</v>
@@ -7319,13 +7318,13 @@
         <v>153</v>
       </c>
       <c r="B172" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C172" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D172" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E172" t="s">
         <v>290</v>
@@ -7348,13 +7347,13 @@
         <v>273</v>
       </c>
       <c r="B173" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="C173" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D173" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E173" t="s">
         <v>290</v>
@@ -7377,13 +7376,13 @@
         <v>137</v>
       </c>
       <c r="B174" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C174" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D174" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E174" t="s">
         <v>290</v>
@@ -7406,13 +7405,13 @@
         <v>146</v>
       </c>
       <c r="B175" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C175" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D175" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E175" t="s">
         <v>290</v>
@@ -7435,7 +7434,7 @@
         <v>134</v>
       </c>
       <c r="B176" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C176" t="s">
         <v>288</v>
@@ -7464,7 +7463,7 @@
         <v>275</v>
       </c>
       <c r="B177" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C177" t="s">
         <v>443</v>
@@ -7493,13 +7492,13 @@
         <v>148</v>
       </c>
       <c r="B178" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C178" t="s">
         <v>264</v>
       </c>
       <c r="D178" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E178" t="s">
         <v>290</v>
@@ -7522,13 +7521,13 @@
         <v>151</v>
       </c>
       <c r="B179" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C179" t="s">
         <v>264</v>
       </c>
       <c r="D179" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E179" t="s">
         <v>290</v>
@@ -7551,13 +7550,13 @@
         <v>274</v>
       </c>
       <c r="B180" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C180" t="s">
         <v>264</v>
       </c>
       <c r="D180" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E180" t="s">
         <v>290</v>
@@ -7580,13 +7579,13 @@
         <v>149</v>
       </c>
       <c r="B181" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C181" t="s">
-        <v>509</v>
-      </c>
-      <c r="D181" t="s">
-        <v>487</v>
+        <v>506</v>
+      </c>
+      <c r="D181" s="4" t="s">
+        <v>520</v>
       </c>
       <c r="E181" t="s">
         <v>290</v>
@@ -7609,13 +7608,13 @@
         <v>129</v>
       </c>
       <c r="B182" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C182" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D182" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="E182" t="s">
         <v>290</v>
@@ -7638,13 +7637,13 @@
         <v>159</v>
       </c>
       <c r="B183" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C183" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D183" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="E183" t="s">
         <v>290</v>
@@ -7667,7 +7666,7 @@
         <v>175</v>
       </c>
       <c r="B184" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C184" t="s">
         <v>295</v>
@@ -7696,7 +7695,7 @@
         <v>176</v>
       </c>
       <c r="B185" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C185" t="s">
         <v>352</v>
@@ -7725,13 +7724,13 @@
         <v>138</v>
       </c>
       <c r="B186" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C186" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D186" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E186" t="s">
         <v>290</v>
@@ -7754,7 +7753,7 @@
         <v>161</v>
       </c>
       <c r="B187" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C187" t="s">
         <v>288</v>
@@ -7783,13 +7782,13 @@
         <v>276</v>
       </c>
       <c r="B188" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C188" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D188" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E188" t="s">
         <v>290</v>
@@ -7809,16 +7808,16 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B189" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C189" t="s">
-        <v>509</v>
-      </c>
-      <c r="D189" t="s">
-        <v>523</v>
+        <v>506</v>
+      </c>
+      <c r="D189" s="4" t="s">
+        <v>520</v>
       </c>
       <c r="E189" t="s">
         <v>290</v>
@@ -7841,13 +7840,13 @@
         <v>147</v>
       </c>
       <c r="B190" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C190" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D190" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="E190" t="s">
         <v>290</v>
@@ -7870,7 +7869,7 @@
         <v>154</v>
       </c>
       <c r="B191" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C191" t="s">
         <v>295</v>
@@ -7899,7 +7898,7 @@
         <v>155</v>
       </c>
       <c r="B192" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C192" t="s">
         <v>355</v>
@@ -7928,7 +7927,7 @@
         <v>163</v>
       </c>
       <c r="B193" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C193" t="s">
         <v>438</v>
@@ -7957,7 +7956,7 @@
         <v>162</v>
       </c>
       <c r="B194" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C194" t="s">
         <v>304</v>
@@ -7986,7 +7985,7 @@
         <v>177</v>
       </c>
       <c r="B195" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C195" t="s">
         <v>381</v>
@@ -8015,13 +8014,13 @@
         <v>164</v>
       </c>
       <c r="B196" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C196" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D196" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E196" t="s">
         <v>290</v>
@@ -8044,7 +8043,7 @@
         <v>172</v>
       </c>
       <c r="B197" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C197" t="s">
         <v>288</v>
@@ -8073,13 +8072,13 @@
         <v>156</v>
       </c>
       <c r="B198" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C198" t="s">
         <v>404</v>
       </c>
       <c r="D198" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E198" t="s">
         <v>290</v>
@@ -8102,7 +8101,7 @@
         <v>173</v>
       </c>
       <c r="B199" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C199" t="s">
         <v>288</v>
@@ -8131,7 +8130,7 @@
         <v>178</v>
       </c>
       <c r="B200" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C200" t="s">
         <v>381</v>
@@ -8160,13 +8159,13 @@
         <v>166</v>
       </c>
       <c r="B201" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C201" t="s">
         <v>288</v>
       </c>
       <c r="D201" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E201" t="s">
         <v>290</v>
@@ -8186,13 +8185,13 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="B202" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C202" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D202" t="s">
         <v>49</v>
@@ -8218,7 +8217,7 @@
         <v>167</v>
       </c>
       <c r="B203" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C203" t="s">
         <v>293</v>
@@ -8247,13 +8246,13 @@
         <v>165</v>
       </c>
       <c r="B204" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C204" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="D204" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="E204" t="s">
         <v>290</v>
@@ -8276,7 +8275,7 @@
         <v>169</v>
       </c>
       <c r="B205" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C205" t="s">
         <v>454</v>
@@ -8305,7 +8304,7 @@
         <v>174</v>
       </c>
       <c r="B206" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C206" t="s">
         <v>288</v>
@@ -8334,7 +8333,7 @@
         <v>158</v>
       </c>
       <c r="B207" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C207" t="s">
         <v>429</v>
@@ -8363,13 +8362,13 @@
         <v>179</v>
       </c>
       <c r="B208" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C208" t="s">
         <v>288</v>
       </c>
       <c r="D208" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E208" t="s">
         <v>290</v>
@@ -8392,13 +8391,13 @@
         <v>157</v>
       </c>
       <c r="B209" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="C209" t="s">
-        <v>550</v>
-      </c>
-      <c r="D209" t="s">
-        <v>469</v>
+        <v>547</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>642</v>
       </c>
       <c r="E209" t="s">
         <v>290</v>
@@ -8421,7 +8420,7 @@
         <v>171</v>
       </c>
       <c r="B210" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C210" t="s">
         <v>288</v>
@@ -8450,13 +8449,13 @@
         <v>170</v>
       </c>
       <c r="B211" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C211" t="s">
-        <v>509</v>
-      </c>
-      <c r="D211" t="s">
-        <v>487</v>
+        <v>506</v>
+      </c>
+      <c r="D211" s="4" t="s">
+        <v>520</v>
       </c>
       <c r="E211" t="s">
         <v>290</v>
@@ -8479,13 +8478,13 @@
         <v>168</v>
       </c>
       <c r="B212" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C212" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D212" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="E212" t="s">
         <v>290</v>
@@ -8508,7 +8507,7 @@
         <v>184</v>
       </c>
       <c r="B213" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C213" t="s">
         <v>295</v>
@@ -8534,10 +8533,10 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B214" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C214" t="s">
         <v>352</v>
@@ -8566,10 +8565,10 @@
         <v>189</v>
       </c>
       <c r="B215" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C215" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D215" t="s">
         <v>310</v>
@@ -8595,13 +8594,13 @@
         <v>190</v>
       </c>
       <c r="B216" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="C216" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D216" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E216" t="s">
         <v>290</v>
@@ -8624,10 +8623,10 @@
         <v>188</v>
       </c>
       <c r="B217" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C217" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="D217" t="s">
         <v>466</v>
@@ -8653,10 +8652,10 @@
         <v>180</v>
       </c>
       <c r="B218" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C218" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D218" t="s">
         <v>431</v>
@@ -8682,10 +8681,10 @@
         <v>186</v>
       </c>
       <c r="B219" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C219" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D219" t="s">
         <v>457</v>
@@ -8711,7 +8710,7 @@
         <v>185</v>
       </c>
       <c r="B220" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C220" t="s">
         <v>293</v>
@@ -8740,13 +8739,13 @@
         <v>187</v>
       </c>
       <c r="B221" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C221" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D221" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E221" t="s">
         <v>290</v>
@@ -8769,7 +8768,7 @@
         <v>183</v>
       </c>
       <c r="B222" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C222" t="s">
         <v>288</v>
@@ -8798,7 +8797,7 @@
         <v>181</v>
       </c>
       <c r="B223" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C223" t="s">
         <v>378</v>
@@ -8827,13 +8826,13 @@
         <v>191</v>
       </c>
       <c r="B224" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="C224" t="s">
         <v>288</v>
       </c>
       <c r="D224" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E224" t="s">
         <v>290</v>
@@ -8856,7 +8855,7 @@
         <v>277</v>
       </c>
       <c r="B225" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C225" t="s">
         <v>293</v>
@@ -8885,13 +8884,13 @@
         <v>182</v>
       </c>
       <c r="B226" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C226" t="s">
-        <v>550</v>
-      </c>
-      <c r="D226" t="s">
-        <v>469</v>
+        <v>547</v>
+      </c>
+      <c r="D226" s="4" t="s">
+        <v>642</v>
       </c>
       <c r="E226" t="s">
         <v>290</v>
@@ -8914,7 +8913,7 @@
         <v>193</v>
       </c>
       <c r="B227" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="C227" t="s">
         <v>288</v>
@@ -8943,10 +8942,10 @@
         <v>198</v>
       </c>
       <c r="B228" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C228" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D228" t="s">
         <v>382</v>
@@ -8972,7 +8971,7 @@
         <v>202</v>
       </c>
       <c r="B229" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C229" t="s">
         <v>443</v>
@@ -9001,7 +9000,7 @@
         <v>192</v>
       </c>
       <c r="B230" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C230" t="s">
         <v>293</v>
@@ -9033,7 +9032,7 @@
         <v>130</v>
       </c>
       <c r="C231" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="D231" t="s">
         <v>310</v>
@@ -9059,7 +9058,7 @@
         <v>282</v>
       </c>
       <c r="B232" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="C232" t="s">
         <v>288</v>
@@ -9088,10 +9087,10 @@
         <v>203</v>
       </c>
       <c r="B233" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C233" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D233" t="s">
         <v>382</v>
@@ -9117,13 +9116,13 @@
         <v>194</v>
       </c>
       <c r="B234" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C234" t="s">
-        <v>586</v>
-      </c>
-      <c r="D234" t="s">
-        <v>469</v>
+        <v>583</v>
+      </c>
+      <c r="D234" s="4" t="s">
+        <v>642</v>
       </c>
       <c r="E234" t="s">
         <v>290</v>
@@ -9146,13 +9145,13 @@
         <v>285</v>
       </c>
       <c r="B235" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="C235" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="D235" t="s">
-        <v>469</v>
+        <v>642</v>
       </c>
       <c r="E235" t="s">
         <v>290</v>
@@ -9175,13 +9174,13 @@
         <v>208</v>
       </c>
       <c r="B236" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="C236" t="s">
-        <v>589</v>
-      </c>
-      <c r="D236" t="s">
-        <v>469</v>
+        <v>586</v>
+      </c>
+      <c r="D236" s="4" t="s">
+        <v>642</v>
       </c>
       <c r="E236" t="s">
         <v>290</v>
@@ -9204,13 +9203,13 @@
         <v>200</v>
       </c>
       <c r="B237" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C237" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="D237" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E237" t="s">
         <v>290</v>
@@ -9233,10 +9232,10 @@
         <v>206</v>
       </c>
       <c r="B238" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="C238" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="D238" t="s">
         <v>310</v>
@@ -9262,10 +9261,10 @@
         <v>195</v>
       </c>
       <c r="B239" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C239" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D239" t="s">
         <v>444</v>
@@ -9291,13 +9290,13 @@
         <v>199</v>
       </c>
       <c r="B240" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C240" t="s">
-        <v>589</v>
-      </c>
-      <c r="D240" t="s">
-        <v>469</v>
+        <v>586</v>
+      </c>
+      <c r="D240" s="4" t="s">
+        <v>642</v>
       </c>
       <c r="E240" t="s">
         <v>290</v>
@@ -9320,10 +9319,10 @@
         <v>201</v>
       </c>
       <c r="B241" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C241" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D241" t="s">
         <v>431</v>
@@ -9349,10 +9348,10 @@
         <v>207</v>
       </c>
       <c r="B242" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C242" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="D242" t="s">
         <v>312</v>
@@ -9378,13 +9377,13 @@
         <v>205</v>
       </c>
       <c r="B243" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C243" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D243" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E243" t="s">
         <v>290</v>
@@ -9407,7 +9406,7 @@
         <v>197</v>
       </c>
       <c r="B244" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C244" t="s">
         <v>293</v>
@@ -9436,7 +9435,7 @@
         <v>196</v>
       </c>
       <c r="B245" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C245" t="s">
         <v>341</v>
@@ -9465,7 +9464,7 @@
         <v>280</v>
       </c>
       <c r="B246" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C246" t="s">
         <v>293</v>
@@ -9494,7 +9493,7 @@
         <v>209</v>
       </c>
       <c r="B247" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="C247" t="s">
         <v>288</v>
@@ -9523,7 +9522,7 @@
         <v>214</v>
       </c>
       <c r="B248" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C248" t="s">
         <v>355</v>
@@ -9552,7 +9551,7 @@
         <v>213</v>
       </c>
       <c r="B249" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="C249" t="s">
         <v>288</v>
@@ -9581,7 +9580,7 @@
         <v>281</v>
       </c>
       <c r="B250" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C250" t="s">
         <v>304</v>
@@ -9610,7 +9609,7 @@
         <v>212</v>
       </c>
       <c r="B251" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="C251" t="s">
         <v>288</v>
@@ -9639,7 +9638,7 @@
         <v>216</v>
       </c>
       <c r="B252" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="C252" t="s">
         <v>288</v>
@@ -9668,7 +9667,7 @@
         <v>283</v>
       </c>
       <c r="B253" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="C253" t="s">
         <v>438</v>
@@ -9697,7 +9696,7 @@
         <v>211</v>
       </c>
       <c r="B254" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="C254" t="s">
         <v>288</v>
@@ -9726,7 +9725,7 @@
         <v>284</v>
       </c>
       <c r="B255" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="C255" t="s">
         <v>288</v>
@@ -9755,7 +9754,7 @@
         <v>210</v>
       </c>
       <c r="B256" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C256" t="s">
         <v>293</v>
@@ -9784,7 +9783,7 @@
         <v>219</v>
       </c>
       <c r="B257" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C257" t="s">
         <v>341</v>
@@ -9813,13 +9812,13 @@
         <v>220</v>
       </c>
       <c r="B258" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C258" t="s">
-        <v>486</v>
-      </c>
-      <c r="D258" t="s">
-        <v>487</v>
+        <v>484</v>
+      </c>
+      <c r="D258" s="4" t="s">
+        <v>646</v>
       </c>
       <c r="E258" t="s">
         <v>290</v>
@@ -9842,7 +9841,7 @@
         <v>215</v>
       </c>
       <c r="B259" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="C259" t="s">
         <v>456</v>
@@ -9871,7 +9870,7 @@
         <v>279</v>
       </c>
       <c r="B260" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C260" t="s">
         <v>302</v>
@@ -9900,7 +9899,7 @@
         <v>278</v>
       </c>
       <c r="B261" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C261" t="s">
         <v>378</v>
@@ -9929,7 +9928,7 @@
         <v>225</v>
       </c>
       <c r="B262" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C262" t="s">
         <v>293</v>
@@ -9958,7 +9957,7 @@
         <v>218</v>
       </c>
       <c r="B263" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="C263" t="s">
         <v>288</v>
@@ -9987,7 +9986,7 @@
         <v>224</v>
       </c>
       <c r="B264" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="C264" t="s">
         <v>288</v>
@@ -10016,13 +10015,13 @@
         <v>222</v>
       </c>
       <c r="B265" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C265" t="s">
         <v>288</v>
       </c>
       <c r="D265" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E265" t="s">
         <v>290</v>
@@ -10045,13 +10044,13 @@
         <v>229</v>
       </c>
       <c r="B266" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C266" t="s">
         <v>288</v>
       </c>
       <c r="D266" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E266" t="s">
         <v>290</v>
@@ -10074,13 +10073,13 @@
         <v>217</v>
       </c>
       <c r="B267" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="C267" t="s">
         <v>264</v>
       </c>
       <c r="D267" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E267" t="s">
         <v>290</v>
@@ -10103,7 +10102,7 @@
         <v>221</v>
       </c>
       <c r="B268" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="C268" t="s">
         <v>288</v>
@@ -10132,7 +10131,7 @@
         <v>223</v>
       </c>
       <c r="B269" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="C269" t="s">
         <v>302</v>
@@ -10161,13 +10160,13 @@
         <v>230</v>
       </c>
       <c r="B270" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C270" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D270" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E270" t="s">
         <v>290</v>
@@ -10190,7 +10189,7 @@
         <v>233</v>
       </c>
       <c r="B271" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="C271" t="s">
         <v>341</v>
@@ -10219,7 +10218,7 @@
         <v>232</v>
       </c>
       <c r="B272" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="C272" t="s">
         <v>288</v>
@@ -10248,7 +10247,7 @@
         <v>227</v>
       </c>
       <c r="B273" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C273" t="s">
         <v>304</v>
@@ -10277,7 +10276,7 @@
         <v>226</v>
       </c>
       <c r="B274" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="C274" t="s">
         <v>288</v>
@@ -10306,13 +10305,13 @@
         <v>231</v>
       </c>
       <c r="B275" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C275" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="D275" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="E275" t="s">
         <v>290</v>
@@ -10335,7 +10334,7 @@
         <v>235</v>
       </c>
       <c r="B276" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C276" t="s">
         <v>302</v>
@@ -10364,10 +10363,10 @@
         <v>286</v>
       </c>
       <c r="B277" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C277" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="D277" t="s">
         <v>310</v>
@@ -10393,7 +10392,7 @@
         <v>234</v>
       </c>
       <c r="B278" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C278" t="s">
         <v>288</v>
@@ -10422,13 +10421,13 @@
         <v>228</v>
       </c>
       <c r="B279" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C279" t="s">
         <v>288</v>
       </c>
       <c r="D279" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E279" t="s">
         <v>290</v>
@@ -10448,16 +10447,16 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="B280" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C280" t="s">
         <v>468</v>
       </c>
       <c r="D280" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="E280" t="s">
         <v>290</v>

</xml_diff>